<commit_message>
Updated 7 test cases for DC Unit scripts with new loading method details
</commit_message>
<xml_diff>
--- a/Test Data/TC_160_Verify Current(DC Units) calculation.xlsx
+++ b/Test Data/TC_160_Verify Current(DC Units) calculation.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FEA21C0-EB95-4EE1-91EA-08FDE0CD70AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Add Devices" sheetId="1" r:id="rId1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
   <si>
     <t>Ancillary Conventional</t>
   </si>
@@ -195,12 +196,18 @@
   </si>
   <si>
     <t>LED Count</t>
+  </si>
+  <si>
+    <t>DC Unit Loading Details Name</t>
+  </si>
+  <si>
+    <t>Current (DC Units)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -257,7 +264,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -280,11 +287,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -309,6 +327,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,6 +421,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -437,6 +473,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -612,11 +665,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -630,11 +683,11 @@
     <col min="7" max="7" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
@@ -643,7 +696,7 @@
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -656,7 +709,7 @@
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -669,7 +722,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -682,14 +735,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>12</v>
       </c>
@@ -717,8 +770,11 @@
       <c r="I7" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J7" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>18</v>
       </c>
@@ -745,6 +801,9 @@
       </c>
       <c r="I8" s="7">
         <v>285.3</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -758,7 +817,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Updated test data for TC-161 and TC-160
</commit_message>
<xml_diff>
--- a/Test Data/TC_160_Verify Current(DC Units) calculation.xlsx
+++ b/Test Data/TC_160_Verify Current(DC Units) calculation.xlsx
@@ -14,8 +14,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="D8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+5B 5" [517.050.017] &amp; 801RIL</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="61">
   <si>
     <t>Ancillary Conventional</t>
   </si>
@@ -62,9 +96,6 @@
     <t>Label</t>
   </si>
   <si>
-    <t>Assign Base/Default Base</t>
-  </si>
-  <si>
     <t>Default DC Units</t>
   </si>
   <si>
@@ -191,9 +222,6 @@
     <t>Row Index</t>
   </si>
   <si>
-    <t>5B 5" [517.050.017] &amp; 801RIL</t>
-  </si>
-  <si>
     <t>LED Count</t>
   </si>
   <si>
@@ -201,13 +229,16 @@
   </si>
   <si>
     <t>Current (DC Units)</t>
+  </si>
+  <si>
+    <t>Assign Base/Default Base Row</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,6 +260,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -630,11 +674,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -718,39 +762,39 @@
         <v>14</v>
       </c>
       <c r="D7" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="H7" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="8" t="s">
+      <c r="I7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>17</v>
-      </c>
       <c r="J7" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="C8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>58</v>
+      <c r="D8" s="11">
+        <v>2</v>
       </c>
       <c r="E8" s="11">
         <v>6</v>
@@ -768,7 +812,7 @@
         <v>285.3</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -778,6 +822,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -799,202 +844,202 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>19</v>
-      </c>
       <c r="C1" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>19</v>
-      </c>
       <c r="C3" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>

</xml_diff>